<commit_message>
Actualizacion script ajuste de temperaturas
</commit_message>
<xml_diff>
--- a/Actividades semillero/Enfriamiento de Newton/datos_temperatura.xlsx
+++ b/Actividades semillero/Enfriamiento de Newton/datos_temperatura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios GitHub\SIMatComPy2025\Actividades semillero\Enfriamiento de Newton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C1A952-2B98-45FB-90B8-C4EC5C1C298B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481192A0-A74C-4440-B681-7760F3BA9259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{537265F9-1EFB-4065-929D-BD98B7893B17}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{537265F9-1EFB-4065-929D-BD98B7893B17}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>t</t>
+    <t>tiempo</t>
   </si>
   <si>
-    <t>T</t>
+    <t>Temperatura</t>
   </si>
 </sst>
 </file>
@@ -419,15 +419,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.90625" style="1"/>
+    <col min="1" max="2" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -443,7 +443,7 @@
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -451,7 +451,7 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -459,7 +459,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>7</v>
       </c>
@@ -467,7 +467,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>9</v>
       </c>

</xml_diff>